<commit_message>
Add tax data for Alabama, to stop the constant alerts!
Standard Deduction still phases out. This is not implemented yet.
</commit_message>
<xml_diff>
--- a/Data Sources/Deductions and Exemptions.xlsx
+++ b/Data Sources/Deductions and Exemptions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minamhere/Dropbox/personal/bryan and chris/Networth/Data Sources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="6220" yWindow="7000" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,6 +126,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -449,10 +459,10 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
@@ -462,7 +472,7 @@
     <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -502,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -522,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -542,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -562,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -582,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -602,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -622,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -642,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -662,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -682,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -702,7 +712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -722,46 +732,89 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
         <v>2015</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="C15">
+        <v>2500</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16">
         <v>2015</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>3750</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17">
         <v>2015</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>7500</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18">
         <v>2015</v>
+      </c>
+      <c r="C18">
+        <v>4700</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -773,13 +826,8 @@
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>